<commit_message>
Update uniform buffer PR and delay reclamation validation
</commit_message>
<xml_diff>
--- a/document/excel_pics/picture_synchronization.xlsx
+++ b/document/excel_pics/picture_synchronization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC20651-6430-4A90-AEDF-B40A5B3A10C4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-10680" yWindow="3285" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10680" yWindow="3285" windowWidth="21600" windowHeight="11385" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>x</t>
   </si>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -614,6 +614,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -645,6 +646,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -652,7 +654,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1470,6 +1471,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1612,6 +1614,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1643,6 +1646,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1650,7 +1654,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2310,6 +2313,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2317,7 +2321,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2921,6 +2924,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2928,7 +2932,861 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.7137034867886694E-2"/>
+          <c:y val="2.8928336620644313E-2"/>
+          <c:w val="0.94963069010313106"/>
+          <c:h val="0.84253749346420459"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Expected walking trip</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet4!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet4!$B$2:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="10">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E00A-43AF-B559-0617FC7D298E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Expected bus trip</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-E00A-43AF-B559-0617FC7D298E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-E00A-43AF-B559-0617FC7D298E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-E00A-43AF-B559-0617FC7D298E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000C-E00A-43AF-B559-0617FC7D298E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet4!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet4!$C$2:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E00A-43AF-B559-0617FC7D298E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual bus trip</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet4!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet4!$D$2:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E00A-43AF-B559-0617FC7D298E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Scheduled bus trip</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-E00A-43AF-B559-0617FC7D298E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-E00A-43AF-B559-0617FC7D298E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet4!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet4!$E$2:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-E00A-43AF-B559-0617FC7D298E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="522952888"/>
+        <c:axId val="522953544"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="522952888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="4"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="522953544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="522953544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="7"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="522952888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.0292979906437315E-2"/>
+          <c:y val="0.89732117804801048"/>
+          <c:w val="0.84153502852496098"/>
+          <c:h val="0.10119948024248449"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3123,6 +3981,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4672,6 +5570,522 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5346,6 +6760,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>276226</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C1B8F7D-0F7F-4BAD-AE99-4BD875EFFD3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5608,7 +7065,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5748,7 +7205,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6198,11 +7655,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6302,4 +7759,198 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0.5</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1.25</v>
+      </c>
+      <c r="C4">
+        <v>0.5</v>
+      </c>
+      <c r="D4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1.25</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1.5</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1.5</v>
+      </c>
+      <c r="C7">
+        <v>1.5</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1.75</v>
+      </c>
+      <c r="C8">
+        <v>1.5</v>
+      </c>
+      <c r="D8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1.75</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>2.5</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>1.5</v>
+      </c>
+      <c r="C12">
+        <v>2.5</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>4.5</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>6.5</v>
+      </c>
+      <c r="C14">
+        <v>6.5</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update high-resolution eps for figure 1 - 6
</commit_message>
<xml_diff>
--- a/document/excel_pics/picture_synchronization.xlsx
+++ b/document/excel_pics/picture_synchronization.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-10680" yWindow="3285" windowWidth="21600" windowHeight="11385" activeTab="3"/>
+    <workbookView xWindow="-10680" yWindow="3285" windowWidth="21600" windowHeight="11385" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>x</t>
   </si>
@@ -3821,6 +3822,631 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.1622860522716354E-2"/>
+          <c:y val="3.9639639639639637E-2"/>
+          <c:w val="0.93343817234113347"/>
+          <c:h val="0.74748329431794003"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet5!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Expected walking trip</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet5!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet5!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3332999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-98A9-4902-A293-AC19263FB4B7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet5!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Expected bus trip</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet5!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet5!$D$2:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-98A9-4902-A293-AC19263FB4B7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet5!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual bus trip</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-98A9-4902-A293-AC19263FB4B7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-98A9-4902-A293-AC19263FB4B7}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet5!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet5!$E$2:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-98A9-4902-A293-AC19263FB4B7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet5!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Scheduled bus trip</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet5!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet5!$F$2:$F$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-98A9-4902-A293-AC19263FB4B7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="522952888"/>
+        <c:axId val="522953544"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="522952888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="6"/>
+          <c:min val="1.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="522953544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="522953544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="7"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="522952888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.0292933869756375E-2"/>
+          <c:y val="0.89974491026459535"/>
+          <c:w val="0.84153502852496098"/>
+          <c:h val="7.2477264666241048E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4021,6 +4647,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -6086,6 +6752,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6803,6 +7985,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C1B8F7D-0F7F-4BAD-AE99-4BD875EFFD3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7765,7 +8990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -7953,4 +9178,125 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>-1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>2.5</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3.3332999999999999</v>
+      </c>
+      <c r="C5">
+        <v>1.5</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>